<commit_message>
Modificari dupa prezentarea de la lab. =>sa fie updateted pentru testare automata
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cerinta" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="118">
   <si>
     <t>…</t>
   </si>
@@ -705,9 +705,6 @@
     <t>1-2T-3-4F-10</t>
   </si>
   <si>
-    <t>1-2T-3-4T-5T-6-7-8-9-10</t>
-  </si>
-  <si>
     <t>Angajat</t>
   </si>
   <si>
@@ -750,9 +747,6 @@
     <t>1,2,3,4,5,8,9,10</t>
   </si>
   <si>
-    <t>1-2T-3-4T-5F-7-8-9-10</t>
-  </si>
-  <si>
     <t>Functie intiala</t>
   </si>
   <si>
@@ -760,13 +754,31 @@
   </si>
   <si>
     <t>Bogdan;Vrajitoarea;134567891234;ASISTENT;15000.0;28</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>1-2T-3-4T-5F-7-8-4F-9-10</t>
+  </si>
+  <si>
+    <t>1-2T-3-4T-5T-6-7-8-4F-9-10</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>1,2,10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -992,6 +1004,14 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1492,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1626,6 +1646,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1653,6 +1679,18 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1662,9 +1700,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1692,14 +1727,62 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1716,68 +1799,41 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1806,9 +1862,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1848,38 +1901,14 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2679,7 +2708,7 @@
   </sheetPr>
   <dimension ref="B1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -2687,12 +2716,12 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="11"/>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="2:17">
       <c r="L2" s="12" t="s">
@@ -2703,33 +2732,33 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="L3" s="65" t="s">
+      <c r="L3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="66"/>
-      <c r="N3" s="67" t="s">
+      <c r="M3" s="68"/>
+      <c r="N3" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="69"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="71"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1">
       <c r="B4" s="1"/>
-      <c r="L4" s="70" t="s">
+      <c r="L4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="70"/>
+      <c r="M4" s="72"/>
       <c r="N4" s="17" t="s">
         <v>71</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="67">
+      <c r="P4" s="69">
         <v>1211</v>
       </c>
-      <c r="Q4" s="69"/>
+      <c r="Q4" s="71"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="1"/>
@@ -2814,7 +2843,7 @@
       </c>
     </row>
     <row r="20" spans="2:2" ht="15" customHeight="1">
-      <c r="B20" s="148" t="s">
+      <c r="B20" s="65" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2838,8 +2867,8 @@
   </sheetPr>
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20:R20"/>
+    <sheetView topLeftCell="D4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2859,56 +2888,56 @@
   <sheetData>
     <row r="1" spans="2:18">
       <c r="B1" s="20"/>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75"/>
     </row>
     <row r="2" spans="2:18">
       <c r="C2" s="22"/>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="73"/>
-      <c r="G5" s="71" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="G5" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="O5" s="89" t="s">
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="O5" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
       <c r="G7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="87" t="s">
+      <c r="O7" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
       <c r="R7" s="24">
         <v>4</v>
       </c>
@@ -2925,11 +2954,11 @@
       <c r="G8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="87" t="s">
+      <c r="O8" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
       <c r="R8" s="24">
         <f>10-8+2</f>
         <v>4</v>
@@ -2944,22 +2973,22 @@
       </c>
       <c r="D9" s="63"/>
       <c r="E9" s="64"/>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="80"/>
-      <c r="O9" s="87" t="s">
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="85"/>
+      <c r="O9" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="87" t="s">
+      <c r="P9" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="87"/>
+      <c r="Q9" s="79"/>
       <c r="R9" s="24">
         <v>4</v>
       </c>
@@ -2973,13 +3002,13 @@
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="64"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="83"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="88"/>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="25">
@@ -2990,13 +3019,13 @@
       </c>
       <c r="D11" s="63"/>
       <c r="E11" s="64"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="83"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="88"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="25">
@@ -3007,19 +3036,19 @@
       </c>
       <c r="D12" s="63"/>
       <c r="E12" s="64"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="83"/>
-      <c r="O12" s="89" t="s">
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="88"/>
+      <c r="O12" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="25">
@@ -3030,13 +3059,13 @@
       </c>
       <c r="D13" s="63"/>
       <c r="E13" s="64"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="83"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="88"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="25">
@@ -3047,21 +3076,21 @@
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="64"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="83"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="88"/>
       <c r="O14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P14" s="88" t="s">
+      <c r="P14" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="88"/>
-      <c r="R14" s="88"/>
+      <c r="Q14" s="76"/>
+      <c r="R14" s="76"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="25">
@@ -3072,13 +3101,13 @@
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="64"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="83"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="88"/>
       <c r="O15" s="26" t="s">
         <v>44</v>
       </c>
@@ -3097,13 +3126,13 @@
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="64"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="83"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="88"/>
       <c r="O16" s="26" t="s">
         <v>45</v>
       </c>
@@ -3122,18 +3151,18 @@
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="64"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="83"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="88"/>
       <c r="O17" s="26" t="s">
         <v>82</v>
       </c>
       <c r="P17" s="77" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q17" s="77"/>
       <c r="R17" s="77"/>
@@ -3144,18 +3173,18 @@
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="64"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="83"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="88"/>
       <c r="O18" s="53" t="s">
         <v>83</v>
       </c>
       <c r="P18" s="77" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="Q18" s="77"/>
       <c r="R18" s="77"/>
@@ -3167,13 +3196,13 @@
       <c r="C19" s="58"/>
       <c r="D19" s="59"/>
       <c r="E19" s="60"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="83"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="88"/>
       <c r="O19" s="19"/>
       <c r="P19" s="77"/>
       <c r="Q19" s="77"/>
@@ -3186,13 +3215,13 @@
       <c r="C20" s="58"/>
       <c r="D20" s="59"/>
       <c r="E20" s="60"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="83"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="88"/>
       <c r="O20" s="27"/>
       <c r="P20" s="77"/>
       <c r="Q20" s="77"/>
@@ -3205,13 +3234,13 @@
       <c r="C21" s="58"/>
       <c r="D21" s="59"/>
       <c r="E21" s="60"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="88"/>
       <c r="O21" s="19"/>
       <c r="P21" s="77"/>
       <c r="Q21" s="77"/>
@@ -3224,13 +3253,13 @@
       <c r="C22" s="58"/>
       <c r="D22" s="59"/>
       <c r="E22" s="60"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="83"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="88"/>
       <c r="O22" s="19"/>
       <c r="P22" s="77"/>
       <c r="Q22" s="77"/>
@@ -3240,86 +3269,75 @@
       <c r="B23" s="25">
         <v>16</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="76"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="85"/>
-      <c r="L23" s="85"/>
-      <c r="M23" s="86"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="25">
         <v>17</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="25">
         <v>18</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="82"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="25">
         <v>19</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="76"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="25">
         <v>20</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="76"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="25">
         <v>21</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="76"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="82"/>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="25">
         <v>22</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="76"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="25">
         <v>23</v>
       </c>
-      <c r="C30" s="74"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="76"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="C7:E7"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C30:E30"/>
@@ -3336,6 +3354,17 @@
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3350,8 +3379,8 @@
   </sheetPr>
   <dimension ref="B1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3383,14 +3412,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="2:24">
       <c r="H2" s="18" t="s">
@@ -3398,15 +3427,15 @@
       </c>
     </row>
     <row r="3" spans="2:24">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="114"/>
       <c r="I3" s="30"/>
       <c r="K3" s="30"/>
     </row>
@@ -3417,139 +3446,139 @@
       <c r="E5" s="29"/>
     </row>
     <row r="6" spans="2:24" ht="15.6">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="95" t="s">
+      <c r="D6" s="103"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="94" t="s">
+      <c r="G6" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
-      <c r="R6" s="94"/>
-      <c r="S6" s="94"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="94"/>
-      <c r="W6" s="94"/>
-      <c r="X6" s="94"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="115"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="115"/>
+      <c r="Q6" s="115"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="115"/>
+      <c r="T6" s="115"/>
+      <c r="U6" s="115"/>
+      <c r="V6" s="115"/>
+      <c r="W6" s="115"/>
+      <c r="X6" s="115"/>
     </row>
     <row r="7" spans="2:24" ht="15.6">
-      <c r="B7" s="94"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="97" t="s">
+      <c r="B7" s="115"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="99" t="s">
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100" t="s">
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="100"/>
-      <c r="X7" s="100"/>
+      <c r="S7" s="92"/>
+      <c r="T7" s="92"/>
+      <c r="U7" s="92"/>
+      <c r="V7" s="92"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="92"/>
     </row>
     <row r="8" spans="2:24" ht="15.6" customHeight="1">
-      <c r="B8" s="94"/>
-      <c r="C8" s="95" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="101" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="95" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="101" t="s">
+      <c r="B8" s="115"/>
+      <c r="C8" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="97"/>
-      <c r="H8" s="115" t="s">
+      <c r="G8" s="116"/>
+      <c r="H8" s="96" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115" t="s">
-        <v>97</v>
-      </c>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="115"/>
-      <c r="N8" s="99" t="s">
+      <c r="M8" s="96"/>
+      <c r="N8" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="99" t="s">
+      <c r="O8" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="99" t="s">
+      <c r="P8" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="99" t="s">
+      <c r="Q8" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="R8" s="100">
+      <c r="R8" s="92">
         <v>0</v>
       </c>
-      <c r="S8" s="100">
+      <c r="S8" s="92">
         <v>1</v>
       </c>
-      <c r="T8" s="100">
+      <c r="T8" s="92">
         <v>2</v>
       </c>
-      <c r="U8" s="100" t="s">
+      <c r="U8" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="100" t="s">
+      <c r="V8" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="W8" s="100" t="s">
+      <c r="W8" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="100" t="s">
+      <c r="X8" s="92" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.6">
-      <c r="B9" s="94"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="97"/>
+      <c r="B9" s="115"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="116"/>
       <c r="H9" s="32" t="s">
         <v>26</v>
       </c>
@@ -3568,17 +3597,17 @@
       <c r="M9" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="99"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="100"/>
-      <c r="W9" s="100"/>
-      <c r="X9" s="100"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="92"/>
+      <c r="S9" s="92"/>
+      <c r="T9" s="92"/>
+      <c r="U9" s="92"/>
+      <c r="V9" s="92"/>
+      <c r="W9" s="92"/>
+      <c r="X9" s="92"/>
     </row>
     <row r="10" spans="2:24" ht="15.6">
       <c r="B10" s="33" t="s">
@@ -3588,41 +3617,47 @@
         <v>27</v>
       </c>
       <c r="D10" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>104</v>
-      </c>
       <c r="F10" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>101</v>
       </c>
       <c r="I10" s="36"/>
       <c r="J10" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="K10" s="36"/>
+        <v>100</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>100</v>
+      </c>
       <c r="L10" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="M10" s="36"/>
+        <v>100</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>100</v>
+      </c>
       <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="37" t="s">
+        <v>100</v>
+      </c>
       <c r="P10" s="37"/>
       <c r="Q10" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R10" s="38"/>
       <c r="S10" s="38"/>
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
       <c r="V10" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W10" s="38"/>
       <c r="X10" s="38"/>
@@ -3631,39 +3666,41 @@
       <c r="B11" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="149" t="s">
+      <c r="C11" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>107</v>
-      </c>
       <c r="F11" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L11" s="36"/>
       <c r="M11" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="O11" s="37" t="s">
+        <v>100</v>
+      </c>
       <c r="P11" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="37"/>
       <c r="R11" s="38"/>
@@ -3671,48 +3708,48 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
       <c r="V11" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W11" s="38"/>
       <c r="X11" s="38"/>
     </row>
     <row r="12" spans="2:24" ht="15.6">
       <c r="B12" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="61">
         <v>28</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="35"/>
+        <v>102</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>112</v>
+      </c>
       <c r="H12" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I12" s="36"/>
-      <c r="J12" s="36" t="s">
-        <v>101</v>
-      </c>
+      <c r="J12" s="36"/>
       <c r="K12" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L12" s="36"/>
       <c r="M12" s="36"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P12" s="37"/>
       <c r="Q12" s="37"/>
       <c r="R12" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -3722,23 +3759,41 @@
       <c r="X12" s="38"/>
     </row>
     <row r="13" spans="2:24" ht="15.6">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
+      <c r="B13" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>117</v>
+      </c>
       <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="I13" s="36" t="s">
+        <v>100</v>
+      </c>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
-      <c r="N13" s="37"/>
+      <c r="N13" s="37" t="s">
+        <v>100</v>
+      </c>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
-      <c r="R13" s="38"/>
+      <c r="R13" s="38" t="s">
+        <v>100</v>
+      </c>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
@@ -3782,82 +3837,72 @@
       <c r="E16" s="29"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="113" t="s">
+      <c r="B18" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
       <c r="E18" s="57"/>
-      <c r="F18" s="114" t="s">
+      <c r="F18" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
-      <c r="L18" s="114"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="95"/>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
-      <c r="F19" s="112" t="s">
+      <c r="F19" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
-      <c r="F20" s="109" t="s">
+      <c r="F20" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="111"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="110"/>
     </row>
     <row r="23" spans="2:12">
       <c r="F23" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:12">
       <c r="F24" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:12">
       <c r="F25" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="C6:E7"/>
     <mergeCell ref="F20:L20"/>
     <mergeCell ref="R8:R9"/>
@@ -3874,9 +3919,19 @@
     <mergeCell ref="X8:X9"/>
     <mergeCell ref="V8:V9"/>
     <mergeCell ref="W8:W9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3890,8 +3945,8 @@
   </sheetPr>
   <dimension ref="B1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3912,40 +3967,40 @@
     <row r="1" spans="2:15" ht="15" customHeight="1">
       <c r="B1" s="11"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="124" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="142" t="s">
+      <c r="E4" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="143"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="2:15" ht="15" thickBot="1">
-      <c r="B5" s="141"/>
-      <c r="C5" s="145"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="125"/>
       <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
@@ -3964,13 +4019,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="E6" s="151" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="150" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="31.2">
@@ -3981,13 +4036,13 @@
         <v>2</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="E7" s="152" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="150" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="31.2">
@@ -3998,21 +4053,29 @@
         <v>3</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="E8" s="152" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="150" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.6">
       <c r="B9" s="3"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="152" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="150" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="10" spans="2:15" ht="16.2" thickBot="1">
       <c r="B10" s="5"/>
@@ -4048,83 +4111,83 @@
       <c r="O13" s="21"/>
     </row>
     <row r="14" spans="2:15" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120" t="s">
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="121"/>
-      <c r="H14" s="118" t="s">
+      <c r="G14" s="133"/>
+      <c r="H14" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="122"/>
-      <c r="M14" s="123" t="s">
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="N14" s="124"/>
+      <c r="N14" s="136"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickTop="1">
-      <c r="B15" s="125" t="s">
+      <c r="B15" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="127" t="s">
+      <c r="C15" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="127" t="s">
+      <c r="D15" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="129" t="s">
+      <c r="E15" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="117" t="s">
+      <c r="F15" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="132" t="s">
+      <c r="G15" s="143" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="133" t="s">
+      <c r="H15" s="144" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="127" t="s">
+      <c r="I15" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="127" t="s">
+      <c r="J15" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="135" t="s">
+      <c r="K15" s="146" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="137" t="s">
+      <c r="L15" s="148" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="139" t="s">
+      <c r="M15" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="N15" s="116" t="s">
+      <c r="N15" s="128" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="25.8" customHeight="1">
-      <c r="B16" s="126"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="128"/>
-      <c r="J16" s="128"/>
-      <c r="K16" s="136"/>
-      <c r="L16" s="138"/>
-      <c r="M16" s="125"/>
-      <c r="N16" s="117"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="139"/>
+      <c r="K16" s="147"/>
+      <c r="L16" s="149"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="129"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="48">
@@ -4138,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="44">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F17" s="45"/>
       <c r="G17" s="46" t="s">
@@ -4171,12 +4234,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="N15:N16"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="F14:G14"/>
@@ -4193,6 +4250,12 @@
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4200,21 +4263,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005276E578212D6F4DAC13DE2BDB632D99" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95b503bd88e770708ece5f67e0ac593f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b852056b-7bae-4ed5-8da6-ebb18f6eced8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a129b49b9ab64774807da9d6a5f31d9" ns2:_="">
     <xsd:import namespace="b852056b-7bae-4ed5-8da6-ebb18f6eced8"/>
@@ -4346,24 +4394,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B74BF37-79AC-4B36-AA3F-5C8A48A04908}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4776DE-C19A-4E88-8C8E-1114DE8D1713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E026628D-90E0-4BF2-B9C8-DFD59B8A8DA5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4379,4 +4425,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4776DE-C19A-4E88-8C8E-1114DE8D1713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B74BF37-79AC-4B36-AA3F-5C8A48A04908}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>